<commit_message>
Unittests geschrieben. Alle laufen
</commit_message>
<xml_diff>
--- a/src/test/testdaten_insert_gemeldete_krankenkasse/gemeldete Krankenkasse.xlsx
+++ b/src/test/testdaten_insert_gemeldete_krankenkasse/gemeldete Krankenkasse.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\main\Sozialversicherungsdaten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxfr\PycharmProjects\Personalstammdatenbank\src\test\testdaten_insert_gemeldete_krankenkasse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3128A9CE-5F79-450E-8BA7-6B243A1F66C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1302EB55-49BA-4586-847D-A9B15CD7CCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="1860" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -389,7 +389,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>